<commit_message>
Cleaned repo. separated munsell functions into separate file, and added convex hulls to plots
</commit_message>
<xml_diff>
--- a/raw material survey data.xlsx
+++ b/raw material survey data.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jon Paige\Desktop\LBJ Attribute analysis\LBJ attribute analysis repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6379DE8C-B749-4F0A-ABC6-783C5D656297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CAE311-B636-4CA8-9EC5-4769BE7F9901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2172" yWindow="1812" windowWidth="19560" windowHeight="8724" xr2:uid="{69B49FDD-EDF3-439C-8B9D-6B0CC6E4D670}"/>
+    <workbookView xWindow="2172" yWindow="1812" windowWidth="19560" windowHeight="8724" firstSheet="2" activeTab="3" xr2:uid="{69B49FDD-EDF3-439C-8B9D-6B0CC6E4D670}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sample measurements" sheetId="2" r:id="rId3"/>
+    <sheet name="Glossary" sheetId="6" r:id="rId4"/>
+    <sheet name="Sample color measurements" sheetId="5" r:id="rId5"/>
+    <sheet name="Heat treatment exp." sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="116">
   <si>
     <t>Locality</t>
   </si>
@@ -139,12 +142,6 @@
     <t>Artifact type</t>
   </si>
   <si>
-    <t>Color measurement location</t>
-  </si>
-  <si>
-    <t>Location description</t>
-  </si>
-  <si>
     <t>Chalky</t>
   </si>
   <si>
@@ -230,16 +227,184 @@
   </si>
   <si>
     <t>3.2.23</t>
+  </si>
+  <si>
+    <t>flk</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>Soak time 120</t>
+  </si>
+  <si>
+    <t>soak time 220</t>
+  </si>
+  <si>
+    <t>Soak time 320</t>
+  </si>
+  <si>
+    <t>Soak time 420</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>mass grams</t>
+  </si>
+  <si>
+    <t>Grain</t>
+  </si>
+  <si>
+    <t>Gloss</t>
+  </si>
+  <si>
+    <t>color 1</t>
+  </si>
+  <si>
+    <t>Color 1.loc</t>
+  </si>
+  <si>
+    <t>Interiormost</t>
+  </si>
+  <si>
+    <t>7.5yr5/2</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>2.2.1</t>
+  </si>
+  <si>
+    <t>Artifact</t>
+  </si>
+  <si>
+    <t>ID description.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Each id's first number is the locality sampled (1-5 were visited, but samples only collected from 2,3 and 5). </t>
+  </si>
+  <si>
+    <t>Each id's second number is the cobble number collected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the third number is the number assigned to a flake taken from that cobble, or a chunk/core remaining after reduction. </t>
+  </si>
+  <si>
+    <t>Munsell estimate</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>5y4/2</t>
+  </si>
+  <si>
+    <t>5y5/2</t>
+  </si>
+  <si>
+    <t>2.5y5/2</t>
+  </si>
+  <si>
+    <t>5yr6/1</t>
+  </si>
+  <si>
+    <t>10yr7/1</t>
+  </si>
+  <si>
+    <t>interiormost</t>
+  </si>
+  <si>
+    <t>exteriormost</t>
+  </si>
+  <si>
+    <t>Finish</t>
+  </si>
+  <si>
+    <t>Translucency</t>
+  </si>
+  <si>
+    <t>opaque</t>
+  </si>
+  <si>
+    <t>2.2.2</t>
+  </si>
+  <si>
+    <t>5yr4/2</t>
+  </si>
+  <si>
+    <t>7.5yr6/2</t>
+  </si>
+  <si>
+    <t>Location of color samples</t>
+  </si>
+  <si>
+    <t>In taking multiple munsell estimates for each sample, I aimed to sample the extremes of the color variation by targeting the interiormost portion of the cobble the flake captured, and the exteriormost.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In cases where the exterior was cortical, I sampled just inside the cortex, to sample color variation where cryptocrystaline chert began. </t>
+  </si>
+  <si>
+    <t>2.2.3</t>
+  </si>
+  <si>
+    <t>7.5r6/2</t>
+  </si>
+  <si>
+    <t>2.5yr5/2</t>
+  </si>
+  <si>
+    <t>5yr7/2</t>
+  </si>
+  <si>
+    <t>5yr7/1</t>
+  </si>
+  <si>
+    <t>2.2.4</t>
+  </si>
+  <si>
+    <t>2.5y5/1</t>
+  </si>
+  <si>
+    <t>10yr5/2</t>
+  </si>
+  <si>
+    <t>5yr5/1</t>
+  </si>
+  <si>
+    <t>proximal</t>
+  </si>
+  <si>
+    <t>distal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in flakes where there was no difference in in the proximity to an interior across the flake, or no discernable color gradient, the general location of the color samples is described. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -583,11 +748,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A70794D5-8754-4185-8149-19A4560E35EF}">
   <dimension ref="A1:S14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -603,7 +771,7 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F1" t="s">
         <v>7</v>
@@ -621,7 +789,7 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L1" t="s">
         <v>10</v>
@@ -630,22 +798,22 @@
         <v>11</v>
       </c>
       <c r="N1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P1" t="s">
         <v>47</v>
       </c>
-      <c r="O1" t="s">
-        <v>48</v>
-      </c>
-      <c r="P1" t="s">
-        <v>49</v>
-      </c>
       <c r="Q1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="R1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="S1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -659,13 +827,13 @@
         <v>87</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
         <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s">
         <v>23</v>
@@ -674,7 +842,7 @@
         <v>22</v>
       </c>
       <c r="I2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J2" t="s">
         <v>23</v>
@@ -683,10 +851,10 @@
         <v>23</v>
       </c>
       <c r="L2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="M2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="N2">
         <v>196</v>
@@ -712,16 +880,16 @@
         <v>87</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
         <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N3">
         <v>133</v>
@@ -747,16 +915,16 @@
         <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
         <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N4">
         <v>102</v>
@@ -782,16 +950,16 @@
         <v>87</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
         <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="N5">
         <v>67.099999999999994</v>
@@ -814,16 +982,16 @@
         <v>3.1</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
         <v>23</v>
       </c>
       <c r="I6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="N6">
         <v>88.6</v>
@@ -846,16 +1014,16 @@
         <v>3.2</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
         <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G7" t="s">
         <v>22</v>
@@ -864,7 +1032,7 @@
         <v>23</v>
       </c>
       <c r="I7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J7" t="s">
         <v>22</v>
@@ -891,7 +1059,7 @@
         <v>0.2</v>
       </c>
       <c r="S7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
@@ -902,19 +1070,19 @@
         <v>3.3</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
         <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="N8">
         <v>58.2</v>
@@ -937,22 +1105,22 @@
         <v>3.4</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
         <v>22</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G9" t="s">
         <v>22</v>
       </c>
       <c r="I9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N9">
         <v>36.5</v>
@@ -975,19 +1143,19 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E10" t="s">
         <v>23</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="N10">
         <v>118</v>
@@ -1010,19 +1178,19 @@
         <v>5.2</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E11" t="s">
         <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N11">
         <v>124.3</v>
@@ -1045,19 +1213,19 @@
         <v>5.3</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
         <v>23</v>
       </c>
       <c r="F12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N12">
         <v>140</v>
@@ -1080,19 +1248,19 @@
         <v>5.4</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E13" t="s">
         <v>23</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="N13">
         <v>170</v>
@@ -1107,7 +1275,7 @@
         <v>1.52</v>
       </c>
       <c r="S13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
@@ -1118,19 +1286,19 @@
         <v>5.5</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E14" t="s">
         <v>23</v>
       </c>
       <c r="F14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N14">
         <v>113</v>
@@ -1194,7 +1362,7 @@
         <v>9</v>
       </c>
       <c r="J1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K1" t="s">
         <v>10</v>
@@ -1217,7 +1385,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
         <v>22</v>
@@ -1232,7 +1400,7 @@
         <v>19</v>
       </c>
       <c r="J2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K2" t="s">
         <v>15</v>
@@ -1243,13 +1411,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
         <v>23</v>
       </c>
       <c r="G3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H3" t="s">
         <v>27</v>
@@ -1258,7 +1426,7 @@
         <v>20</v>
       </c>
       <c r="J3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K3" t="s">
         <v>16</v>
@@ -1269,13 +1437,13 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H4" t="s">
         <v>28</v>
@@ -1292,7 +1460,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H5" t="s">
         <v>29</v>
@@ -1308,22 +1476,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48341863-B27B-4B2A-9D16-2738324A3EAB}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.6640625" customWidth="1"/>
     <col min="2" max="2" width="11.77734375" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="31.6640625" customWidth="1"/>
-    <col min="5" max="5" width="28.21875" customWidth="1"/>
+    <col min="3" max="9" width="13.33203125" customWidth="1"/>
+    <col min="10" max="10" width="8.21875" customWidth="1"/>
+    <col min="11" max="11" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -1334,13 +1502,712 @@
         <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>70</v>
+      </c>
+      <c r="F1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2">
+        <v>32.4</v>
+      </c>
+      <c r="E2">
+        <v>14.9</v>
+      </c>
+      <c r="F2">
+        <v>3.9</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" t="s">
+        <v>78</v>
+      </c>
+      <c r="K2" t="s">
+        <v>77</v>
+      </c>
+      <c r="L2" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DC8848-191B-42B2-8890-F216156A1F30}">
+  <dimension ref="A2:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B40DD1-8598-4DD1-8579-BBC3335FDF4F}">
+  <dimension ref="A1:G25"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" t="s">
+        <v>97</v>
+      </c>
+      <c r="G8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" t="s">
+        <v>97</v>
+      </c>
+      <c r="G9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" t="s">
+        <v>97</v>
+      </c>
+      <c r="G11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" t="s">
+        <v>97</v>
+      </c>
+      <c r="G13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" t="s">
+        <v>97</v>
+      </c>
+      <c r="G14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" t="s">
+        <v>97</v>
+      </c>
+      <c r="G16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" t="s">
+        <v>97</v>
+      </c>
+      <c r="G17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" t="s">
+        <v>97</v>
+      </c>
+      <c r="G19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" t="s">
+        <v>97</v>
+      </c>
+      <c r="G20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>111</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" t="s">
+        <v>97</v>
+      </c>
+      <c r="G21" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" t="s">
+        <v>97</v>
+      </c>
+      <c r="G22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" t="s">
+        <v>97</v>
+      </c>
+      <c r="G23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F24" t="s">
+        <v>97</v>
+      </c>
+      <c r="G24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" t="s">
+        <v>97</v>
+      </c>
+      <c r="G25" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04DCAAE7-6A9E-4EAB-AD8E-DD6BE22A8E92}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>